<commit_message>
Atualização automática de TEUTONIA.xlsx
</commit_message>
<xml_diff>
--- a/TEUTONIA.xlsx
+++ b/TEUTONIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{136DF137-00AC-4A1D-88A8-68906358FA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DB2581E-6990-4E92-AC47-34BBCE28D85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1308,7 +1308,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{13C7C652-0C10-4CAF-B0EC-0DDC289C0D68}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{4670706E-FE56-42E3-B18E-1920132DD5C8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1338,10 +1338,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC679432-86D0-4DE5-B40B-C51DD8A010E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F05BF6EE-32F8-469F-8A0A-82CB98C76C89}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1379,7 +1379,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ED1D57F-B59A-4964-AD89-C4AAFFD4DAD3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2596B9B2-0109-4E24-A55D-A9F70CA854BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1442,7 +1442,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{151C92C4-EA9D-431C-AFEC-1B95B105E0E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E931277-AE9F-413C-99E0-B19F2197C459}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1461,7 +1461,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96450731-1790-EB0C-E4B3-C11CC04597E1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BACD9F-75DB-E61B-7FDC-1AEDBF041826}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1510,7 +1510,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51F43893-E843-D90B-99E4-184962CF0709}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6F4342B-FC00-C3A3-E5D2-5E23A4ED08CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1529,7 +1529,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF62338D-A6AB-9729-013A-7EAB14318BF5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDD54E45-5A5C-3B34-18A3-46849189F2DA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1560,7 +1560,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8898589B-29B8-D5BF-5A17-35AEA78D7511}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B95BB2E9-286A-17BE-7FBC-3F03EE6670B8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1591,7 +1591,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82129EA6-F647-5ED6-600E-31ED1AFA5E60}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DBA898C-5A1A-58DE-DF6C-D96549D2563D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1634,7 +1634,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8857DA09-1D8C-4AFF-A8D4-9C1EF2DF9D2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E5339D-CAEB-4197-9DA2-8BB3D5122C32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1672,7 +1672,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F636888-DF5D-4A0A-81E4-B64B2DEE2D68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1D00169-26FB-46AC-B2FF-5F9A696376C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1715,7 +1715,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D64406A2-BBE8-4513-9DC7-0631E60143CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6956CDF-8447-4594-A703-30429C28F20C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2028,7 +2028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE2C17E-81E6-4401-9E94-BC945511AC52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6814295-A583-4678-BA3E-2C57EBDF3A59}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>